<commit_message>
fix to multigraph and update dbs
</commit_message>
<xml_diff>
--- a/Learning_to_Route/raw results.xlsx
+++ b/Learning_to_Route/raw results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Research_Implementing\Learning_to_Route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1444244-8FAF-4DFD-9FDD-D22219547867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443266E7-E6AD-40D1-860C-32E9C4AADE3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40356033-B3A7-46B4-97A9-44C2D2D1AC68}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40356033-B3A7-46B4-97A9-44C2D2D1AC68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>1.27</v>
+        <v>1.28</v>
       </c>
       <c r="G22" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
fix reports and graphs
</commit_message>
<xml_diff>
--- a/Learning_to_Route/raw results.xlsx
+++ b/Learning_to_Route/raw results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Research_Implementing\Learning_to_Route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5D1F0C-C86E-485D-8425-9B9AF6EAF6C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E637B72B-7E4C-4495-9A1F-DBD7882C0F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{40356033-B3A7-46B4-97A9-44C2D2D1AC68}"/>
+    <workbookView xWindow="-15345" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{40356033-B3A7-46B4-97A9-44C2D2D1AC68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,14 +415,16 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -467,8 +469,14 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1.59</v>
+      </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1.26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -481,8 +489,14 @@
       <c r="D7">
         <v>3</v>
       </c>
+      <c r="E7">
+        <v>1.47</v>
+      </c>
       <c r="G7">
         <v>3</v>
+      </c>
+      <c r="H7">
+        <v>1.18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -495,8 +509,14 @@
       <c r="D8">
         <v>5</v>
       </c>
+      <c r="E8">
+        <v>1.4</v>
+      </c>
       <c r="G8">
         <v>5</v>
+      </c>
+      <c r="H8">
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -509,9 +529,15 @@
       <c r="D9">
         <v>10</v>
       </c>
+      <c r="E9">
+        <v>1.35</v>
+      </c>
       <c r="G9">
         <v>10</v>
       </c>
+      <c r="H9">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -523,8 +549,14 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
+      <c r="E10">
+        <v>1.2</v>
+      </c>
       <c r="G10" t="s">
         <v>3</v>
+      </c>
+      <c r="H10">
+        <v>1.2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -562,55 +594,100 @@
       <c r="A18">
         <v>1</v>
       </c>
+      <c r="B18">
+        <v>1.2</v>
+      </c>
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18">
+        <v>1.19</v>
+      </c>
       <c r="G18">
         <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1.17</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
+      <c r="B19">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="D19">
         <v>3</v>
       </c>
+      <c r="E19">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="G19">
         <v>3</v>
+      </c>
+      <c r="H19">
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>5</v>
       </c>
+      <c r="B20">
+        <v>1.07</v>
+      </c>
       <c r="D20">
         <v>5</v>
       </c>
+      <c r="E20">
+        <v>1.07</v>
+      </c>
       <c r="G20">
         <v>5</v>
+      </c>
+      <c r="H20">
+        <v>1.07</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
+      <c r="B21">
+        <v>1.06</v>
+      </c>
       <c r="D21">
         <v>10</v>
       </c>
+      <c r="E21">
+        <v>1.06</v>
+      </c>
       <c r="G21">
         <v>10</v>
       </c>
+      <c r="H21">
+        <v>1.06</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>
+      <c r="B22">
+        <v>1.0900000000000001</v>
+      </c>
       <c r="D22" t="s">
         <v>3</v>
       </c>
+      <c r="E22">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="G22" t="s">
         <v>3</v>
+      </c>
+      <c r="H22">
+        <v>1.1299999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>